<commit_message>
Paper Writing: Performing more experiments
</commit_message>
<xml_diff>
--- a/Synthetic/Result.xlsx
+++ b/Synthetic/Result.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1stLevel" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2ndLevel" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="FirstOrder-Old" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="SecondOrder-Old" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ROC-Alpha" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ROC-Magnitude" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="44">
   <si>
     <t xml:space="preserve">Centralized</t>
   </si>
@@ -218,6 +220,84 @@
     <t xml:space="preserve">3.5σ
 [0.03~0.05]</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Level Cen</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Level Equ</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ν=0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ν=0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ν=0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ν=0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ν=1.0</t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK SC Regular"/>
@@ -291,8 +371,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +408,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -365,7 +458,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,7 +467,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,6 +567,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -553,15 +662,15 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="23:23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="2" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="2" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.1581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,13 +2498,13 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="23:23 A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4203,17 +4312,17 @@
   </sheetPr>
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="1" sqref="23:23 P8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="12.6632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="5.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="5.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="12.6632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="14.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="5.62244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.4642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="5.62244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.4642857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5270,24 +5379,24 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="1" sqref="23:23 Q13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.72448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="5.72448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.0663265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.53571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="6.53571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.4489795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.4489795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.4489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6059,4 +6168,4599 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AE47"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="2" style="0" width="6.12755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="8.83673469387755"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="N1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="Z1" s="28"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">B4/(B4+E4)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">C4/(C4+D4)</f>
+        <v>0.164794007490637</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">H4/(H4+K4)</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">I4/(I4+J4)</f>
+        <v>0.18957345971564</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">N4/(N4+Q4)</f>
+        <v>1</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <f aca="false">O4/(O4+P4)</f>
+        <v>0.160839160839161</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <f aca="false">T4/(T4+W4)</f>
+        <v>1</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <f aca="false">U4/(U4+V4)</f>
+        <v>0.0441176470588235</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>264</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <f aca="false">Z4/(Z4+AC4)</f>
+        <v>1</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <f aca="false">AA4/(AA4+AB4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">B5/(B5+E5)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">C5/(C5+D5)</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">H5/(H5+K5)</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">I5/(I5+J5)</f>
+        <v>0.163366336633663</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">N5/(N5+Q5)</f>
+        <v>1</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false">O5/(O5+P5)</f>
+        <v>0.164179104477612</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <f aca="false">T5/(T5+W5)</f>
+        <v>1</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <f aca="false">U5/(U5+V5)</f>
+        <v>0.104166666666667</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <f aca="false">Z5/(Z5+AC5)</f>
+        <v>1</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <f aca="false">AA5/(AA5+AB5)</f>
+        <v>0.228571428571429</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">B6/(B6+E6)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">C6/(C6+D6)</f>
+        <v>0.162878787878788</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">H6/(H6+K6)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">I6/(I6+J6)</f>
+        <v>0.157142857142857</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <f aca="false">N6/(N6+Q6)</f>
+        <v>1</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <f aca="false">O6/(O6+P6)</f>
+        <v>0.153846153846154</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <f aca="false">T6/(T6+W6)</f>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <f aca="false">U6/(U6+V6)</f>
+        <v>0.164835164835165</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <f aca="false">Z6/(Z6+AC6)</f>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <f aca="false">AA6/(AA6+AB6)</f>
+        <v>0.153846153846154</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="29" t="n">
+        <f aca="false">AVERAGE(F4:F6)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="29" t="n">
+        <f aca="false">AVERAGE(G4:G6)</f>
+        <v>0.164779820678697</v>
+      </c>
+      <c r="L7" s="29" t="n">
+        <f aca="false">AVERAGE(L4:L6)</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="29" t="n">
+        <f aca="false">AVERAGE(M4:M6)</f>
+        <v>0.170027551164053</v>
+      </c>
+      <c r="R7" s="29" t="n">
+        <f aca="false">AVERAGE(R4:R6)</f>
+        <v>1</v>
+      </c>
+      <c r="S7" s="29" t="n">
+        <f aca="false">AVERAGE(S4:S6)</f>
+        <v>0.159621473054309</v>
+      </c>
+      <c r="X7" s="29" t="n">
+        <f aca="false">AVERAGE(X4:X6)</f>
+        <v>1</v>
+      </c>
+      <c r="Y7" s="29" t="n">
+        <f aca="false">AVERAGE(Y4:Y6)</f>
+        <v>0.104373159520218</v>
+      </c>
+      <c r="AD7" s="29" t="n">
+        <f aca="false">AVERAGE(AD4:AD6)</f>
+        <v>1</v>
+      </c>
+      <c r="AE7" s="29" t="n">
+        <f aca="false">AVERAGE(AE4:AE6)</f>
+        <v>0.127472527472527</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>253</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">B8/(B8+E8)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">C8/(C8+D8)</f>
+        <v>0.0193798449612403</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">H8/(H8+K8)</f>
+        <v>0.978494623655914</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">I8/(I8+J8)</f>
+        <v>0.0148514851485149</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">N8/(N8+Q8)</f>
+        <v>0.992481203007519</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <f aca="false">O8/(O8+P8)</f>
+        <v>0.0123456790123457</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <f aca="false">T8/(T8+W8)</f>
+        <v>0.980952380952381</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <f aca="false">U8/(U8+V8)</f>
+        <v>0.0117647058823529</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <f aca="false">Z8/(Z8+AC8)</f>
+        <v>0.956043956043956</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <f aca="false">AA8/(AA8+AB8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">B9/(B9+E9)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">C9/(C9+D9)</f>
+        <v>0.01953125</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">H9/(H9+K9)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">I9/(I9+J9)</f>
+        <v>0.0192307692307692</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">N9/(N9+Q9)</f>
+        <v>0.993197278911565</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <f aca="false">O9/(O9+P9)</f>
+        <v>0.00675675675675676</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <f aca="false">T9/(T9+W9)</f>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <f aca="false">U9/(U9+V9)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <f aca="false">Z9/(Z9+AC9)</f>
+        <v>0.969811320754717</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <f aca="false">AA9/(AA9+AB9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">B10/(B10+E10)</f>
+        <v>0.96875</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">C10/(C10+D10)</f>
+        <v>0.0152091254752852</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">H10/(H10+K10)</f>
+        <v>0.988636363636364</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">I10/(I10+J10)</f>
+        <v>0.00966183574879227</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">N10/(N10+Q10)</f>
+        <v>0.992805755395684</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <f aca="false">O10/(O10+P10)</f>
+        <v>0.0256410256410256</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <f aca="false">T10/(T10+W10)</f>
+        <v>0.990610328638498</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <f aca="false">U10/(U10+V10)</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>262</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <f aca="false">Z10/(Z10+AC10)</f>
+        <v>0.984962406015038</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <f aca="false">AA10/(AA10+AB10)</f>
+        <v>0.0689655172413793</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="29" t="n">
+        <f aca="false">AVERAGE(F8:F10)</f>
+        <v>0.989583333333333</v>
+      </c>
+      <c r="G11" s="29" t="n">
+        <f aca="false">AVERAGE(G8:G10)</f>
+        <v>0.0180400734788418</v>
+      </c>
+      <c r="L11" s="29" t="n">
+        <f aca="false">AVERAGE(L8:L10)</f>
+        <v>0.989043662430759</v>
+      </c>
+      <c r="M11" s="29" t="n">
+        <f aca="false">AVERAGE(M8:M10)</f>
+        <v>0.0145813633760255</v>
+      </c>
+      <c r="R11" s="29" t="n">
+        <f aca="false">AVERAGE(R8:R10)</f>
+        <v>0.992828079104922</v>
+      </c>
+      <c r="S11" s="29" t="n">
+        <f aca="false">AVERAGE(S8:S10)</f>
+        <v>0.0149144871367094</v>
+      </c>
+      <c r="X11" s="29" t="n">
+        <f aca="false">AVERAGE(X8:X10)</f>
+        <v>0.990520903196959</v>
+      </c>
+      <c r="Y11" s="29" t="n">
+        <f aca="false">AVERAGE(Y8:Y10)</f>
+        <v>0.00392156862745098</v>
+      </c>
+      <c r="AD11" s="29" t="n">
+        <f aca="false">AVERAGE(AD8:AD10)</f>
+        <v>0.970272560937904</v>
+      </c>
+      <c r="AE11" s="29" t="n">
+        <f aca="false">AVERAGE(AE8:AE10)</f>
+        <v>0.0229885057471264</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">B12/(B12+E12)</f>
+        <v>0.875</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">C12/(C12+D12)</f>
+        <v>0.003690036900369</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">H12/(H12+K12)</f>
+        <v>0.857142857142857</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">I12/(I12+J12)</f>
+        <v>0.00490196078431373</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">N12/(N12+Q12)</f>
+        <v>0.792207792207792</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <f aca="false">O12/(O12+P12)</f>
+        <v>0.0212765957446808</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <f aca="false">T12/(T12+W12)</f>
+        <v>0.703517587939699</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <f aca="false">U12/(U12+V12)</f>
+        <v>0.0104166666666667</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="AD12" s="0" t="n">
+        <f aca="false">Z12/(Z12+AC12)</f>
+        <v>0.680769230769231</v>
+      </c>
+      <c r="AE12" s="0" t="n">
+        <f aca="false">AA12/(AA12+AB12)</f>
+        <v>0.0285714285714286</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">B13/(B13+E13)</f>
+        <v>0.785714285714286</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">C13/(C13+D13)</f>
+        <v>0.00749063670411985</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">H13/(H13+K13)</f>
+        <v>0.808080808080808</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">I13/(I13+J13)</f>
+        <v>0.0102040816326531</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">N13/(N13+Q13)</f>
+        <v>0.732484076433121</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <f aca="false">O13/(O13+P13)</f>
+        <v>0.0072463768115942</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <f aca="false">T13/(T13+W13)</f>
+        <v>0.701570680628272</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <f aca="false">U13/(U13+V13)</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC13" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="AD13" s="0" t="n">
+        <f aca="false">Z13/(Z13+AC13)</f>
+        <v>0.691449814126394</v>
+      </c>
+      <c r="AE13" s="0" t="n">
+        <f aca="false">AA13/(AA13+AB13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">B14/(B14+E14)</f>
+        <v>0.823529411764706</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">C14/(C14+D14)</f>
+        <v>0.00766283524904215</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">H14/(H14+K14)</f>
+        <v>0.817073170731707</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">I14/(I14+J14)</f>
+        <v>0.00469483568075117</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">N14/(N14+Q14)</f>
+        <v>0.789473684210526</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <f aca="false">O14/(O14+P14)</f>
+        <v>0.013986013986014</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <f aca="false">T14/(T14+W14)</f>
+        <v>0.744897959183674</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <f aca="false">U14/(U14+V14)</f>
+        <v>0.0202020202020202</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC14" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="AD14" s="0" t="n">
+        <f aca="false">Z14/(Z14+AC14)</f>
+        <v>0.687022900763359</v>
+      </c>
+      <c r="AE14" s="0" t="n">
+        <f aca="false">AA14/(AA14+AB14)</f>
+        <v>0.0909090909090909</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="29" t="n">
+        <f aca="false">AVERAGE(F12:F14)</f>
+        <v>0.828081232492997</v>
+      </c>
+      <c r="G15" s="29" t="n">
+        <f aca="false">AVERAGE(G12:G14)</f>
+        <v>0.00628116961784367</v>
+      </c>
+      <c r="L15" s="29" t="n">
+        <f aca="false">AVERAGE(L12:L14)</f>
+        <v>0.827432278651791</v>
+      </c>
+      <c r="M15" s="29" t="n">
+        <f aca="false">AVERAGE(M12:M14)</f>
+        <v>0.00660029269923932</v>
+      </c>
+      <c r="R15" s="29" t="n">
+        <f aca="false">AVERAGE(R12:R14)</f>
+        <v>0.771388517617146</v>
+      </c>
+      <c r="S15" s="29" t="n">
+        <f aca="false">AVERAGE(S12:S14)</f>
+        <v>0.014169662180763</v>
+      </c>
+      <c r="X15" s="29" t="n">
+        <f aca="false">AVERAGE(X12:X14)</f>
+        <v>0.716662075917215</v>
+      </c>
+      <c r="Y15" s="29" t="n">
+        <f aca="false">AVERAGE(Y12:Y14)</f>
+        <v>0.010206228956229</v>
+      </c>
+      <c r="AD15" s="29" t="n">
+        <f aca="false">AVERAGE(AD12:AD14)</f>
+        <v>0.686413981886328</v>
+      </c>
+      <c r="AE15" s="29" t="n">
+        <f aca="false">AVERAGE(AE12:AE14)</f>
+        <v>0.0398268398268398</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">B16/(B16+E16)</f>
+        <v>0.555555555555556</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">C16/(C16+D16)</f>
+        <v>0.00772200772200772</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>208</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">H16/(H16+K16)</f>
+        <v>0.395348837209302</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">I16/(I16+J16)</f>
+        <v>0.00478468899521531</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">N16/(N16+Q16)</f>
+        <v>0.531645569620253</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <f aca="false">O16/(O16+P16)</f>
+        <v>0.0072992700729927</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <f aca="false">T16/(T16+W16)</f>
+        <v>0.487562189054726</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <f aca="false">U16/(U16+V16)</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <f aca="false">Z16/(Z16+AC16)</f>
+        <v>0.515037593984962</v>
+      </c>
+      <c r="AE16" s="0" t="n">
+        <f aca="false">AA16/(AA16+AB16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">B17/(B17+E17)</f>
+        <v>0.444444444444444</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">C17/(C17+D17)</f>
+        <v>0.00772200772200772</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">H17/(H17+K17)</f>
+        <v>0.430379746835443</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">I17/(I17+J17)</f>
+        <v>0.00925925925925926</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">N17/(N17+Q17)</f>
+        <v>0.776699029126214</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <f aca="false">O17/(O17+P17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <f aca="false">T17/(T17+W17)</f>
+        <v>0.446153846153846</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <f aca="false">U17/(U17+V17)</f>
+        <v>0.02</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <f aca="false">Z17/(Z17+AC17)</f>
+        <v>0.480769230769231</v>
+      </c>
+      <c r="AE17" s="0" t="n">
+        <f aca="false">AA17/(AA17+AB17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">B18/(B18+E18)</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">C18/(C18+D18)</f>
+        <v>0.00760456273764259</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">H18/(H18+K18)</f>
+        <v>0.447058823529412</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <f aca="false">I18/(I18+J18)</f>
+        <v>0.00476190476190476</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <f aca="false">N18/(N18+Q18)</f>
+        <v>0.429530201342282</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <f aca="false">O18/(O18+P18)</f>
+        <v>0.00684931506849315</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <f aca="false">T18/(T18+W18)</f>
+        <v>0.483870967741936</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <f aca="false">U18/(U18+V18)</f>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <f aca="false">Z18/(Z18+AC18)</f>
+        <v>0.503703703703704</v>
+      </c>
+      <c r="AE18" s="0" t="n">
+        <f aca="false">AA18/(AA18+AB18)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="29" t="n">
+        <f aca="false">AVERAGE(F16:F18)</f>
+        <v>0.555555555555556</v>
+      </c>
+      <c r="G19" s="29" t="n">
+        <f aca="false">AVERAGE(G16:G18)</f>
+        <v>0.00768285939388601</v>
+      </c>
+      <c r="L19" s="29" t="n">
+        <f aca="false">AVERAGE(L16:L18)</f>
+        <v>0.424262469191386</v>
+      </c>
+      <c r="M19" s="29" t="n">
+        <f aca="false">AVERAGE(M16:M18)</f>
+        <v>0.00626861767212644</v>
+      </c>
+      <c r="R19" s="29" t="n">
+        <f aca="false">AVERAGE(R16:R18)</f>
+        <v>0.579291600029583</v>
+      </c>
+      <c r="S19" s="29" t="n">
+        <f aca="false">AVERAGE(S16:S18)</f>
+        <v>0.00471619504716195</v>
+      </c>
+      <c r="X19" s="29" t="n">
+        <f aca="false">AVERAGE(X16:X18)</f>
+        <v>0.472529000983503</v>
+      </c>
+      <c r="Y19" s="29" t="n">
+        <f aca="false">AVERAGE(Y16:Y18)</f>
+        <v>0.00666666666666667</v>
+      </c>
+      <c r="AD19" s="29" t="n">
+        <f aca="false">AVERAGE(AD16:AD18)</f>
+        <v>0.499836842819299</v>
+      </c>
+      <c r="AE19" s="29" t="n">
+        <f aca="false">AVERAGE(AE16:AE18)</f>
+        <v>0.0133333333333333</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">B20/(B20+E20)</f>
+        <v>0.256410256410256</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">C20/(C20+D20)</f>
+        <v>0.0037593984962406</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">H20/(H20+K20)</f>
+        <v>0.25974025974026</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">I20/(I20+J20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <f aca="false">N20/(N20+Q20)</f>
+        <v>0.314102564102564</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <f aca="false">O20/(O20+P20)</f>
+        <v>0.00719424460431655</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <f aca="false">T20/(T20+W20)</f>
+        <v>0.271428571428571</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <f aca="false">U20/(U20+V20)</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC20" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="AD20" s="0" t="n">
+        <f aca="false">Z20/(Z20+AC20)</f>
+        <v>0.314606741573034</v>
+      </c>
+      <c r="AE20" s="0" t="n">
+        <f aca="false">AA20/(AA20+AB20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>262</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">B21/(B21+E21)</f>
+        <v>0.28125</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">C21/(C21+D21)</f>
+        <v>0.00380228136882129</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">H21/(H21+K21)</f>
+        <v>0.311827956989247</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <f aca="false">I21/(I21+J21)</f>
+        <v>0.00495049504950495</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <f aca="false">N21/(N21+Q21)</f>
+        <v>0.278571428571429</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <f aca="false">O21/(O21+P21)</f>
+        <v>0.00645161290322581</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <f aca="false">T21/(T21+W21)</f>
+        <v>0.307692307692308</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <f aca="false">U21/(U21+V21)</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC21" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="AD21" s="0" t="n">
+        <f aca="false">Z21/(Z21+AC21)</f>
+        <v>0.337121212121212</v>
+      </c>
+      <c r="AE21" s="0" t="n">
+        <f aca="false">AA21/(AA21+AB21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">B22/(B22+E22)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">C22/(C22+D22)</f>
+        <v>0.003690036900369</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">H22/(H22+K22)</f>
+        <v>0.269230769230769</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <f aca="false">I22/(I22+J22)</f>
+        <v>0.00460829493087558</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <f aca="false">N22/(N22+Q22)</f>
+        <v>0.25</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <f aca="false">O22/(O22+P22)</f>
+        <v>0.00628930817610063</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <f aca="false">T22/(T22+W22)</f>
+        <v>0.248730964467005</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <f aca="false">U22/(U22+V22)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <f aca="false">Z22/(Z22+AC22)</f>
+        <v>0.302238805970149</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <f aca="false">AA22/(AA22+AB22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="29" t="n">
+        <f aca="false">AVERAGE(F20:F22)</f>
+        <v>0.262553418803419</v>
+      </c>
+      <c r="G23" s="29" t="n">
+        <f aca="false">AVERAGE(G20:G22)</f>
+        <v>0.00375057225514363</v>
+      </c>
+      <c r="L23" s="29" t="n">
+        <f aca="false">AVERAGE(L20:L22)</f>
+        <v>0.280266328653425</v>
+      </c>
+      <c r="M23" s="29" t="n">
+        <f aca="false">AVERAGE(M20:M22)</f>
+        <v>0.00318626332679351</v>
+      </c>
+      <c r="R23" s="29" t="n">
+        <f aca="false">AVERAGE(R20:R22)</f>
+        <v>0.280891330891331</v>
+      </c>
+      <c r="S23" s="29" t="n">
+        <f aca="false">AVERAGE(S20:S22)</f>
+        <v>0.006645055227881</v>
+      </c>
+      <c r="X23" s="29" t="n">
+        <f aca="false">AVERAGE(X20:X22)</f>
+        <v>0.275950614529295</v>
+      </c>
+      <c r="Y23" s="29" t="n">
+        <f aca="false">AVERAGE(Y20:Y22)</f>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="29" t="n">
+        <f aca="false">AVERAGE(AD20:AD22)</f>
+        <v>0.317988919888132</v>
+      </c>
+      <c r="AE23" s="29" t="n">
+        <f aca="false">AVERAGE(AE20:AE22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="N25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="Z25" s="28"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA26" s="27"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="27"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="X27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE27" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">B28/(B28+E28)</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">C28/(C28+D28)</f>
+        <v>0.376425855513308</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <f aca="false">H28/(H28+K28)</f>
+        <v>1</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <f aca="false">I28/(I28+J28)</f>
+        <v>0.386138613861386</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <f aca="false">N28/(N28+Q28)</f>
+        <v>1</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <f aca="false">O28/(O28+P28)</f>
+        <v>0.356687898089172</v>
+      </c>
+      <c r="T28" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="U28" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="V28" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="W28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" s="0" t="n">
+        <f aca="false">T28/(T28+W28)</f>
+        <v>1</v>
+      </c>
+      <c r="Y28" s="0" t="n">
+        <f aca="false">U28/(U28+V28)</f>
+        <v>0.351648351648352</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <f aca="false">Z28/(Z28+AC28)</f>
+        <v>1</v>
+      </c>
+      <c r="AE28" s="0" t="n">
+        <f aca="false">AA28/(AA28+AB28)</f>
+        <v>0.346153846153846</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="F29" s="0" t="e">
+        <f aca="false">B29/(B29+E29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="0" t="e">
+        <f aca="false">C29/(C29+D29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L29" s="0" t="e">
+        <f aca="false">H29/(H29+K29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="0" t="e">
+        <f aca="false">I29/(I29+J29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R29" s="0" t="e">
+        <f aca="false">N29/(N29+Q29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S29" s="0" t="e">
+        <f aca="false">O29/(O29+P29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X29" s="0" t="e">
+        <f aca="false">T29/(T29+W29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y29" s="0" t="e">
+        <f aca="false">U29/(U29+V29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD29" s="0" t="e">
+        <f aca="false">Z29/(Z29+AC29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE29" s="0" t="e">
+        <f aca="false">AA29/(AA29+AB29)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2"/>
+      <c r="F30" s="0" t="e">
+        <f aca="false">B30/(B30+E30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" s="0" t="e">
+        <f aca="false">C30/(C30+D30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" s="0" t="e">
+        <f aca="false">H30/(H30+K30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30" s="0" t="e">
+        <f aca="false">I30/(I30+J30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R30" s="0" t="e">
+        <f aca="false">N30/(N30+Q30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S30" s="0" t="e">
+        <f aca="false">O30/(O30+P30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X30" s="0" t="e">
+        <f aca="false">T30/(T30+W30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y30" s="0" t="e">
+        <f aca="false">U30/(U30+V30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD30" s="0" t="e">
+        <f aca="false">Z30/(Z30+AC30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE30" s="0" t="e">
+        <f aca="false">AA30/(AA30+AB30)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="29" t="e">
+        <f aca="false">AVERAGE(F28:F30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="29" t="e">
+        <f aca="false">AVERAGE(G28:G30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="29" t="e">
+        <f aca="false">AVERAGE(L28:L30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="29" t="e">
+        <f aca="false">AVERAGE(M28:M30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R31" s="29" t="e">
+        <f aca="false">AVERAGE(R28:R30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S31" s="29" t="e">
+        <f aca="false">AVERAGE(S28:S30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X31" s="29" t="e">
+        <f aca="false">AVERAGE(X28:X30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y31" s="29" t="e">
+        <f aca="false">AVERAGE(Y28:Y30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD31" s="29" t="e">
+        <f aca="false">AVERAGE(AD28:AD30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE31" s="29" t="e">
+        <f aca="false">AVERAGE(AE28:AE30)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">B32/(B32+E32)</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">C32/(C32+D32)</f>
+        <v>0.0641509433962264</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <f aca="false">H32/(H32+K32)</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <f aca="false">I32/(I32+J32)</f>
+        <v>0.0757575757575758</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <f aca="false">N32/(N32+Q32)</f>
+        <v>1</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <f aca="false">O32/(O32+P32)</f>
+        <v>0.107692307692308</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="U32" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="V32" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="W32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" s="0" t="n">
+        <f aca="false">T32/(T32+W32)</f>
+        <v>1</v>
+      </c>
+      <c r="Y32" s="0" t="n">
+        <f aca="false">U32/(U32+V32)</f>
+        <v>0.145833333333333</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="AA32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB32" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="0" t="n">
+        <f aca="false">Z32/(Z32+AC32)</f>
+        <v>1</v>
+      </c>
+      <c r="AE32" s="0" t="n">
+        <f aca="false">AA32/(AA32+AB32)</f>
+        <v>0.111111111111111</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="F33" s="0" t="e">
+        <f aca="false">B33/(B33+E33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33" s="0" t="e">
+        <f aca="false">C33/(C33+D33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L33" s="0" t="e">
+        <f aca="false">H33/(H33+K33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="0" t="e">
+        <f aca="false">I33/(I33+J33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R33" s="0" t="e">
+        <f aca="false">N33/(N33+Q33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S33" s="0" t="e">
+        <f aca="false">O33/(O33+P33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X33" s="0" t="e">
+        <f aca="false">T33/(T33+W33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y33" s="0" t="e">
+        <f aca="false">U33/(U33+V33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD33" s="0" t="e">
+        <f aca="false">Z33/(Z33+AC33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE33" s="0" t="e">
+        <f aca="false">AA33/(AA33+AB33)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="F34" s="0" t="e">
+        <f aca="false">B34/(B34+E34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" s="0" t="e">
+        <f aca="false">C34/(C34+D34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L34" s="0" t="e">
+        <f aca="false">H34/(H34+K34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" s="0" t="e">
+        <f aca="false">I34/(I34+J34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R34" s="0" t="e">
+        <f aca="false">N34/(N34+Q34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S34" s="0" t="e">
+        <f aca="false">O34/(O34+P34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X34" s="0" t="e">
+        <f aca="false">T34/(T34+W34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y34" s="0" t="e">
+        <f aca="false">U34/(U34+V34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD34" s="0" t="e">
+        <f aca="false">Z34/(Z34+AC34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE34" s="0" t="e">
+        <f aca="false">AA34/(AA34+AB34)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="29" t="e">
+        <f aca="false">AVERAGE(F32:F34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="29" t="e">
+        <f aca="false">AVERAGE(G32:G34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" s="29" t="e">
+        <f aca="false">AVERAGE(L32:L34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="29" t="e">
+        <f aca="false">AVERAGE(M32:M34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R35" s="29" t="e">
+        <f aca="false">AVERAGE(R32:R34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S35" s="29" t="e">
+        <f aca="false">AVERAGE(S32:S34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X35" s="29" t="e">
+        <f aca="false">AVERAGE(X32:X34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y35" s="29" t="e">
+        <f aca="false">AVERAGE(Y32:Y34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD35" s="29" t="e">
+        <f aca="false">AVERAGE(AD32:AD34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE35" s="29" t="e">
+        <f aca="false">AVERAGE(AE32:AE34)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">B36/(B36+E36)</f>
+        <v>0.866666666666667</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f aca="false">C36/(C36+D36)</f>
+        <v>0.00754716981132076</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <f aca="false">H36/(H36+K36)</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <f aca="false">I36/(I36+J36)</f>
+        <v>0.0100502512562814</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <f aca="false">N36/(N36+Q36)</f>
+        <v>0.77027027027027</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <f aca="false">O36/(O36+P36)</f>
+        <v>0.0136054421768707</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="U36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V36" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="W36" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="X36" s="0" t="n">
+        <f aca="false">T36/(T36+W36)</f>
+        <v>0.831818181818182</v>
+      </c>
+      <c r="Y36" s="0" t="n">
+        <f aca="false">U36/(U36+V36)</f>
+        <v>0.04</v>
+      </c>
+      <c r="Z36" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="AA36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB36" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="0" t="n">
+        <f aca="false">Z36/(Z36+AC36)</f>
+        <v>1</v>
+      </c>
+      <c r="AE36" s="0" t="n">
+        <f aca="false">AA36/(AA36+AB36)</f>
+        <v>0.0588235294117647</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="F37" s="0" t="e">
+        <f aca="false">B37/(B37+E37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" s="0" t="e">
+        <f aca="false">C37/(C37+D37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L37" s="0" t="e">
+        <f aca="false">H37/(H37+K37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" s="0" t="e">
+        <f aca="false">I37/(I37+J37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R37" s="0" t="e">
+        <f aca="false">N37/(N37+Q37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S37" s="0" t="e">
+        <f aca="false">O37/(O37+P37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X37" s="0" t="e">
+        <f aca="false">T37/(T37+W37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y37" s="0" t="e">
+        <f aca="false">U37/(U37+V37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD37" s="0" t="e">
+        <f aca="false">Z37/(Z37+AC37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE37" s="0" t="e">
+        <f aca="false">AA37/(AA37+AB37)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="F38" s="0" t="e">
+        <f aca="false">B38/(B38+E38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" s="0" t="e">
+        <f aca="false">C38/(C38+D38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L38" s="0" t="e">
+        <f aca="false">H38/(H38+K38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M38" s="0" t="e">
+        <f aca="false">I38/(I38+J38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R38" s="0" t="e">
+        <f aca="false">N38/(N38+Q38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S38" s="0" t="e">
+        <f aca="false">O38/(O38+P38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X38" s="0" t="e">
+        <f aca="false">T38/(T38+W38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y38" s="0" t="e">
+        <f aca="false">U38/(U38+V38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD38" s="0" t="e">
+        <f aca="false">Z38/(Z38+AC38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE38" s="0" t="e">
+        <f aca="false">AA38/(AA38+AB38)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="29" t="e">
+        <f aca="false">AVERAGE(F36:F38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39" s="29" t="e">
+        <f aca="false">AVERAGE(G36:G38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L39" s="29" t="e">
+        <f aca="false">AVERAGE(L36:L38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" s="29" t="e">
+        <f aca="false">AVERAGE(M36:M38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R39" s="29" t="e">
+        <f aca="false">AVERAGE(R36:R38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S39" s="29" t="e">
+        <f aca="false">AVERAGE(S36:S38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X39" s="29" t="e">
+        <f aca="false">AVERAGE(X36:X38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y39" s="29" t="e">
+        <f aca="false">AVERAGE(Y36:Y38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD39" s="29" t="e">
+        <f aca="false">AVERAGE(AD36:AD38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE39" s="29" t="e">
+        <f aca="false">AVERAGE(AE36:AE38)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">B40/(B40+E40)</f>
+        <v>0.655172413793103</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">C40/(C40+D40)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <f aca="false">H40/(H40+K40)</f>
+        <v>0.357142857142857</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <f aca="false">I40/(I40+J40)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <f aca="false">N40/(N40+Q40)</f>
+        <v>0.18796992481203</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <f aca="false">O40/(O40+P40)</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V40" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="X40" s="0" t="n">
+        <f aca="false">T40/(T40+W40)</f>
+        <v>0.0904761904761905</v>
+      </c>
+      <c r="Y40" s="0" t="n">
+        <f aca="false">U40/(U40+V40)</f>
+        <v>0.0470588235294118</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC40" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="AD40" s="0" t="n">
+        <f aca="false">Z40/(Z40+AC40)</f>
+        <v>0.214814814814815</v>
+      </c>
+      <c r="AE40" s="0" t="n">
+        <f aca="false">AA40/(AA40+AB40)</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="F41" s="0" t="e">
+        <f aca="false">B41/(B41+E41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" s="0" t="e">
+        <f aca="false">C41/(C41+D41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L41" s="0" t="e">
+        <f aca="false">H41/(H41+K41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M41" s="0" t="e">
+        <f aca="false">I41/(I41+J41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R41" s="0" t="e">
+        <f aca="false">N41/(N41+Q41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S41" s="0" t="e">
+        <f aca="false">O41/(O41+P41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X41" s="0" t="e">
+        <f aca="false">T41/(T41+W41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y41" s="0" t="e">
+        <f aca="false">U41/(U41+V41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD41" s="0" t="e">
+        <f aca="false">Z41/(Z41+AC41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE41" s="0" t="e">
+        <f aca="false">AA41/(AA41+AB41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+      <c r="F42" s="0" t="e">
+        <f aca="false">B42/(B42+E42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G42" s="0" t="e">
+        <f aca="false">C42/(C42+D42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42" s="0" t="e">
+        <f aca="false">H42/(H42+K42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M42" s="0" t="e">
+        <f aca="false">I42/(I42+J42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R42" s="0" t="e">
+        <f aca="false">N42/(N42+Q42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S42" s="0" t="e">
+        <f aca="false">O42/(O42+P42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X42" s="0" t="e">
+        <f aca="false">T42/(T42+W42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y42" s="0" t="e">
+        <f aca="false">U42/(U42+V42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD42" s="0" t="e">
+        <f aca="false">Z42/(Z42+AC42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE42" s="0" t="e">
+        <f aca="false">AA42/(AA42+AB42)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F43" s="29" t="e">
+        <f aca="false">AVERAGE(F40:F42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" s="29" t="e">
+        <f aca="false">AVERAGE(G40:G42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" s="29" t="e">
+        <f aca="false">AVERAGE(L40:L42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M43" s="29" t="e">
+        <f aca="false">AVERAGE(M40:M42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R43" s="29" t="e">
+        <f aca="false">AVERAGE(R40:R42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S43" s="29" t="e">
+        <f aca="false">AVERAGE(S40:S42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X43" s="29" t="e">
+        <f aca="false">AVERAGE(X40:X42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y43" s="29" t="e">
+        <f aca="false">AVERAGE(Y40:Y42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD43" s="29" t="e">
+        <f aca="false">AVERAGE(AD40:AD42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE43" s="29" t="e">
+        <f aca="false">AVERAGE(AE40:AE42)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">B44/(B44+E44)</f>
+        <v>0.346153846153846</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">C44/(C44+D44)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>213</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <f aca="false">H44/(H44+K44)</f>
+        <v>0.0853658536585366</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <f aca="false">I44/(I44+J44)</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="R44" s="0" t="n">
+        <f aca="false">N44/(N44+Q44)</f>
+        <v>0.0479452054794521</v>
+      </c>
+      <c r="S44" s="0" t="n">
+        <f aca="false">O44/(O44+P44)</f>
+        <v>0</v>
+      </c>
+      <c r="T44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V44" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="W44" s="0" t="n">
+        <v>208</v>
+      </c>
+      <c r="X44" s="0" t="n">
+        <f aca="false">T44/(T44+W44)</f>
+        <v>0.0280373831775701</v>
+      </c>
+      <c r="Y44" s="0" t="n">
+        <f aca="false">U44/(U44+V44)</f>
+        <v>0.0123456790123457</v>
+      </c>
+      <c r="Z44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC44" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="AD44" s="0" t="n">
+        <f aca="false">Z44/(Z44+AC44)</f>
+        <v>0.0150943396226415</v>
+      </c>
+      <c r="AE44" s="0" t="n">
+        <f aca="false">AA44/(AA44+AB44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+      <c r="F45" s="0" t="e">
+        <f aca="false">B45/(B45+E45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45" s="0" t="e">
+        <f aca="false">C45/(C45+D45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="0" t="e">
+        <f aca="false">H45/(H45+K45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" s="0" t="e">
+        <f aca="false">I45/(I45+J45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R45" s="0" t="e">
+        <f aca="false">N45/(N45+Q45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S45" s="0" t="e">
+        <f aca="false">O45/(O45+P45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X45" s="0" t="e">
+        <f aca="false">T45/(T45+W45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y45" s="0" t="e">
+        <f aca="false">U45/(U45+V45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD45" s="0" t="e">
+        <f aca="false">Z45/(Z45+AC45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE45" s="0" t="e">
+        <f aca="false">AA45/(AA45+AB45)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2"/>
+      <c r="F46" s="0" t="e">
+        <f aca="false">B46/(B46+E46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" s="0" t="e">
+        <f aca="false">C46/(C46+D46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="0" t="e">
+        <f aca="false">H46/(H46+K46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" s="0" t="e">
+        <f aca="false">I46/(I46+J46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R46" s="0" t="e">
+        <f aca="false">N46/(N46+Q46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S46" s="0" t="e">
+        <f aca="false">O46/(O46+P46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X46" s="0" t="e">
+        <f aca="false">T46/(T46+W46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y46" s="0" t="e">
+        <f aca="false">U46/(U46+V46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD46" s="0" t="e">
+        <f aca="false">Z46/(Z46+AC46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE46" s="0" t="e">
+        <f aca="false">AA46/(AA46+AB46)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="29" t="e">
+        <f aca="false">AVERAGE(F44:F46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="29" t="e">
+        <f aca="false">AVERAGE(G44:G46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="29" t="e">
+        <f aca="false">AVERAGE(L44:L46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="29" t="e">
+        <f aca="false">AVERAGE(M44:M46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R47" s="29" t="e">
+        <f aca="false">AVERAGE(R44:R46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S47" s="29" t="e">
+        <f aca="false">AVERAGE(S44:S46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X47" s="29" t="e">
+        <f aca="false">AVERAGE(X44:X46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y47" s="29" t="e">
+        <f aca="false">AVERAGE(Y44:Y46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD47" s="29" t="e">
+        <f aca="false">AVERAGE(AD44:AD46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE47" s="29" t="e">
+        <f aca="false">AVERAGE(AE44:AE46)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="Z2:AE2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="N26:S26"/>
+    <mergeCell ref="T26:Y26"/>
+    <mergeCell ref="Z26:AE26"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A44:A46"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:AI24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="7.43367346938776"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="I3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="P3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="W3" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AD3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">B5/(B5+E5)</f>
+        <v>0.904109589041096</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">C5/(C5+D5)</f>
+        <v>0.932885906040268</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M5" s="0" t="e">
+        <f aca="false">I5/(I5+L5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="0" t="e">
+        <f aca="false">J5/(J5+K5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="T5" s="0" t="e">
+        <f aca="false">P5/(P5+S5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" s="0" t="e">
+        <f aca="false">Q5/(Q5+R5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA5" s="0" t="e">
+        <f aca="false">W5/(W5+Z5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB5" s="0" t="e">
+        <f aca="false">X5/(X5+Y5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC5" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AH5" s="0" t="e">
+        <f aca="false">AD5/(AD5+AG5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI5" s="0" t="e">
+        <f aca="false">AE5/(AE5+AF5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">B6/(B6+E6)</f>
+        <v>0.946564885496183</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">C6/(C6+D6)</f>
+        <v>0.853658536585366</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="M6" s="0" t="e">
+        <f aca="false">I6/(I6+L6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="0" t="e">
+        <f aca="false">J6/(J6+K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="T6" s="0" t="e">
+        <f aca="false">P6/(P6+S6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="0" t="e">
+        <f aca="false">Q6/(Q6+R6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="AA6" s="0" t="e">
+        <f aca="false">W6/(W6+Z6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB6" s="0" t="e">
+        <f aca="false">X6/(X6+Y6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC6" s="2"/>
+      <c r="AH6" s="0" t="e">
+        <f aca="false">AD6/(AD6+AG6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI6" s="0" t="e">
+        <f aca="false">AE6/(AE6+AF6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">B7/(B7+E7)</f>
+        <v>0.957142857142857</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">C7/(C7+D7)</f>
+        <v>0.819354838709677</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="M7" s="0" t="e">
+        <f aca="false">I7/(I7+L7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="0" t="e">
+        <f aca="false">J7/(J7+K7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="T7" s="0" t="e">
+        <f aca="false">P7/(P7+S7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U7" s="0" t="e">
+        <f aca="false">Q7/(Q7+R7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="AA7" s="0" t="e">
+        <f aca="false">W7/(W7+Z7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB7" s="0" t="e">
+        <f aca="false">X7/(X7+Y7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC7" s="2"/>
+      <c r="AH7" s="0" t="e">
+        <f aca="false">AD7/(AD7+AG7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI7" s="0" t="e">
+        <f aca="false">AE7/(AE7+AF7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="29" t="n">
+        <f aca="false">AVERAGE(F5:F7)</f>
+        <v>0.935939110560045</v>
+      </c>
+      <c r="G8" s="29" t="n">
+        <f aca="false">AVERAGE(G5:G7)</f>
+        <v>0.868633093778437</v>
+      </c>
+      <c r="M8" s="29" t="e">
+        <f aca="false">AVERAGE(M5:M7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="29" t="e">
+        <f aca="false">AVERAGE(N5:N7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T8" s="29" t="e">
+        <f aca="false">AVERAGE(T5:T7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U8" s="29" t="e">
+        <f aca="false">AVERAGE(U5:U7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA8" s="29" t="e">
+        <f aca="false">AVERAGE(AA5:AA7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB8" s="29" t="e">
+        <f aca="false">AVERAGE(AB5:AB7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH8" s="29" t="e">
+        <f aca="false">AVERAGE(AH5:AH7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI8" s="29" t="e">
+        <f aca="false">AVERAGE(AI5:AI7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">B9/(B9+E9)</f>
+        <v>0.798611111111111</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">C9/(C9+D9)</f>
+        <v>0.470198675496689</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M9" s="0" t="e">
+        <f aca="false">I9/(I9+L9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="0" t="e">
+        <f aca="false">J9/(J9+K9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="T9" s="0" t="e">
+        <f aca="false">P9/(P9+S9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="0" t="e">
+        <f aca="false">Q9/(Q9+R9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AA9" s="0" t="e">
+        <f aca="false">W9/(W9+Z9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="0" t="e">
+        <f aca="false">X9/(X9+Y9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AH9" s="0" t="e">
+        <f aca="false">AD9/(AD9+AG9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI9" s="0" t="e">
+        <f aca="false">AE9/(AE9+AF9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">B10/(B10+E10)</f>
+        <v>0.867088607594937</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">C10/(C10+D10)</f>
+        <v>0.423357664233577</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="M10" s="0" t="e">
+        <f aca="false">I10/(I10+L10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="0" t="e">
+        <f aca="false">J10/(J10+K10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="T10" s="0" t="e">
+        <f aca="false">P10/(P10+S10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U10" s="0" t="e">
+        <f aca="false">Q10/(Q10+R10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="AA10" s="0" t="e">
+        <f aca="false">W10/(W10+Z10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB10" s="0" t="e">
+        <f aca="false">X10/(X10+Y10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC10" s="2"/>
+      <c r="AH10" s="0" t="e">
+        <f aca="false">AD10/(AD10+AG10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI10" s="0" t="e">
+        <f aca="false">AE10/(AE10+AF10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="F11" s="0" t="e">
+        <f aca="false">B11/(B11+E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="0" t="e">
+        <f aca="false">C11/(C11+D11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="M11" s="0" t="e">
+        <f aca="false">I11/(I11+L11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="0" t="e">
+        <f aca="false">J11/(J11+K11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="T11" s="0" t="e">
+        <f aca="false">P11/(P11+S11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U11" s="0" t="e">
+        <f aca="false">Q11/(Q11+R11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="AA11" s="0" t="e">
+        <f aca="false">W11/(W11+Z11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB11" s="0" t="e">
+        <f aca="false">X11/(X11+Y11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC11" s="2"/>
+      <c r="AH11" s="0" t="e">
+        <f aca="false">AD11/(AD11+AG11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI11" s="0" t="e">
+        <f aca="false">AE11/(AE11+AF11)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="29" t="e">
+        <f aca="false">AVERAGE(F9:F11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="29" t="e">
+        <f aca="false">AVERAGE(G9:G11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="29" t="e">
+        <f aca="false">AVERAGE(M9:M11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="29" t="e">
+        <f aca="false">AVERAGE(N9:N11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T12" s="29" t="e">
+        <f aca="false">AVERAGE(T9:T11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12" s="29" t="e">
+        <f aca="false">AVERAGE(U9:U11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA12" s="29" t="e">
+        <f aca="false">AVERAGE(AA9:AA11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB12" s="29" t="e">
+        <f aca="false">AVERAGE(AB9:AB11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH12" s="29" t="e">
+        <f aca="false">AVERAGE(AH9:AH11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI12" s="29" t="e">
+        <f aca="false">AVERAGE(AI9:AI11)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">B13/(B13+E13)</f>
+        <v>0.697841726618705</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">C13/(C13+D13)</f>
+        <v>0.217948717948718</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M13" s="0" t="e">
+        <f aca="false">I13/(I13+L13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="0" t="e">
+        <f aca="false">J13/(J13+K13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="T13" s="0" t="e">
+        <f aca="false">P13/(P13+S13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13" s="0" t="e">
+        <f aca="false">Q13/(Q13+R13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AA13" s="0" t="e">
+        <f aca="false">W13/(W13+Z13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB13" s="0" t="e">
+        <f aca="false">X13/(X13+Y13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC13" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AH13" s="0" t="e">
+        <f aca="false">AD13/(AD13+AG13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI13" s="0" t="e">
+        <f aca="false">AE13/(AE13+AF13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">B14/(B14+E14)</f>
+        <v>0.697183098591549</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">C14/(C14+D14)</f>
+        <v>0.254901960784314</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="M14" s="0" t="e">
+        <f aca="false">I14/(I14+L14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" s="0" t="e">
+        <f aca="false">J14/(J14+K14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="T14" s="0" t="e">
+        <f aca="false">P14/(P14+S14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" s="0" t="e">
+        <f aca="false">Q14/(Q14+R14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="AA14" s="0" t="e">
+        <f aca="false">W14/(W14+Z14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB14" s="0" t="e">
+        <f aca="false">X14/(X14+Y14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC14" s="2"/>
+      <c r="AH14" s="0" t="e">
+        <f aca="false">AD14/(AD14+AG14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI14" s="0" t="e">
+        <f aca="false">AE14/(AE14+AF14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+      <c r="B15" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">B15/(B15+E15)</f>
+        <v>0.690140845070423</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">C15/(C15+D15)</f>
+        <v>0.281045751633987</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="M15" s="0" t="e">
+        <f aca="false">I15/(I15+L15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="0" t="e">
+        <f aca="false">J15/(J15+K15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="T15" s="0" t="e">
+        <f aca="false">P15/(P15+S15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" s="0" t="e">
+        <f aca="false">Q15/(Q15+R15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="AA15" s="0" t="e">
+        <f aca="false">W15/(W15+Z15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB15" s="0" t="e">
+        <f aca="false">X15/(X15+Y15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC15" s="2"/>
+      <c r="AH15" s="0" t="e">
+        <f aca="false">AD15/(AD15+AG15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI15" s="0" t="e">
+        <f aca="false">AE15/(AE15+AF15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="29" t="n">
+        <f aca="false">AVERAGE(F13:F15)</f>
+        <v>0.695055223426892</v>
+      </c>
+      <c r="G16" s="29" t="n">
+        <f aca="false">AVERAGE(G13:G15)</f>
+        <v>0.251298810122339</v>
+      </c>
+      <c r="M16" s="29" t="e">
+        <f aca="false">AVERAGE(M13:M15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="29" t="e">
+        <f aca="false">AVERAGE(N13:N15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T16" s="29" t="e">
+        <f aca="false">AVERAGE(T13:T15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="29" t="e">
+        <f aca="false">AVERAGE(U13:U15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA16" s="29" t="e">
+        <f aca="false">AVERAGE(AA13:AA15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB16" s="29" t="e">
+        <f aca="false">AVERAGE(AB13:AB15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH16" s="29" t="e">
+        <f aca="false">AVERAGE(AH13:AH15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI16" s="29" t="e">
+        <f aca="false">AVERAGE(AI13:AI15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">B17/(B17+E17)</f>
+        <v>0.420118343195266</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">C17/(C17+D17)</f>
+        <v>0.0555555555555556</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M17" s="0" t="e">
+        <f aca="false">I17/(I17+L17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" s="0" t="e">
+        <f aca="false">J17/(J17+K17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="T17" s="0" t="e">
+        <f aca="false">P17/(P17+S17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="0" t="e">
+        <f aca="false">Q17/(Q17+R17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AA17" s="0" t="e">
+        <f aca="false">W17/(W17+Z17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB17" s="0" t="e">
+        <f aca="false">X17/(X17+Y17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC17" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AH17" s="0" t="e">
+        <f aca="false">AD17/(AD17+AG17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI17" s="0" t="e">
+        <f aca="false">AE17/(AE17+AF17)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">B18/(B18+E18)</f>
+        <v>0.452054794520548</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">C18/(C18+D18)</f>
+        <v>0.0469798657718121</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="M18" s="0" t="e">
+        <f aca="false">I18/(I18+L18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="0" t="e">
+        <f aca="false">J18/(J18+K18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="T18" s="0" t="e">
+        <f aca="false">P18/(P18+S18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U18" s="0" t="e">
+        <f aca="false">Q18/(Q18+R18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V18" s="2"/>
+      <c r="AA18" s="0" t="e">
+        <f aca="false">W18/(W18+Z18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB18" s="0" t="e">
+        <f aca="false">X18/(X18+Y18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC18" s="2"/>
+      <c r="AH18" s="0" t="e">
+        <f aca="false">AD18/(AD18+AG18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI18" s="0" t="e">
+        <f aca="false">AE18/(AE18+AF18)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">B19/(B19+E19)</f>
+        <v>0.437086092715232</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">C19/(C19+D19)</f>
+        <v>0.0763888888888889</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="M19" s="0" t="e">
+        <f aca="false">I19/(I19+L19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="0" t="e">
+        <f aca="false">J19/(J19+K19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="T19" s="0" t="e">
+        <f aca="false">P19/(P19+S19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="0" t="e">
+        <f aca="false">Q19/(Q19+R19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="AA19" s="0" t="e">
+        <f aca="false">W19/(W19+Z19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB19" s="0" t="e">
+        <f aca="false">X19/(X19+Y19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC19" s="2"/>
+      <c r="AH19" s="0" t="e">
+        <f aca="false">AD19/(AD19+AG19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI19" s="0" t="e">
+        <f aca="false">AE19/(AE19+AF19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="29" t="n">
+        <f aca="false">AVERAGE(F17:F19)</f>
+        <v>0.436419743477015</v>
+      </c>
+      <c r="G20" s="29" t="n">
+        <f aca="false">AVERAGE(G17:G19)</f>
+        <v>0.0596414367387522</v>
+      </c>
+      <c r="M20" s="29" t="e">
+        <f aca="false">AVERAGE(M17:M19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="29" t="e">
+        <f aca="false">AVERAGE(N17:N19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" s="29" t="e">
+        <f aca="false">AVERAGE(T17:T19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="29" t="e">
+        <f aca="false">AVERAGE(U17:U19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA20" s="29" t="e">
+        <f aca="false">AVERAGE(AA17:AA19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB20" s="29" t="e">
+        <f aca="false">AVERAGE(AB17:AB19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH20" s="29" t="e">
+        <f aca="false">AVERAGE(AH17:AH19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI20" s="29" t="e">
+        <f aca="false">AVERAGE(AI17:AI19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="F21" s="0" t="e">
+        <f aca="false">B21/(B21+E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="0" t="e">
+        <f aca="false">C21/(C21+D21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M21" s="0" t="e">
+        <f aca="false">I21/(I21+L21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="0" t="e">
+        <f aca="false">J21/(J21+K21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="T21" s="0" t="e">
+        <f aca="false">P21/(P21+S21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="0" t="e">
+        <f aca="false">Q21/(Q21+R21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AA21" s="0" t="e">
+        <f aca="false">W21/(W21+Z21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB21" s="0" t="e">
+        <f aca="false">X21/(X21+Y21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC21" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AH21" s="0" t="e">
+        <f aca="false">AD21/(AD21+AG21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI21" s="0" t="e">
+        <f aca="false">AE21/(AE21+AF21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="F22" s="0" t="e">
+        <f aca="false">B22/(B22+E22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="0" t="e">
+        <f aca="false">C22/(C22+D22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="M22" s="0" t="e">
+        <f aca="false">I22/(I22+L22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="0" t="e">
+        <f aca="false">J22/(J22+K22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="T22" s="0" t="e">
+        <f aca="false">P22/(P22+S22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="0" t="e">
+        <f aca="false">Q22/(Q22+R22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V22" s="2"/>
+      <c r="AA22" s="0" t="e">
+        <f aca="false">W22/(W22+Z22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB22" s="0" t="e">
+        <f aca="false">X22/(X22+Y22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC22" s="2"/>
+      <c r="AH22" s="0" t="e">
+        <f aca="false">AD22/(AD22+AG22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI22" s="0" t="e">
+        <f aca="false">AE22/(AE22+AF22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="F23" s="0" t="e">
+        <f aca="false">B23/(B23+E23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="0" t="e">
+        <f aca="false">C23/(C23+D23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="M23" s="0" t="e">
+        <f aca="false">I23/(I23+L23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="0" t="e">
+        <f aca="false">J23/(J23+K23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="T23" s="0" t="e">
+        <f aca="false">P23/(P23+S23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="0" t="e">
+        <f aca="false">Q23/(Q23+R23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V23" s="2"/>
+      <c r="AA23" s="0" t="e">
+        <f aca="false">W23/(W23+Z23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB23" s="0" t="e">
+        <f aca="false">X23/(X23+Y23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC23" s="2"/>
+      <c r="AH23" s="0" t="e">
+        <f aca="false">AD23/(AD23+AG23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI23" s="0" t="e">
+        <f aca="false">AE23/(AE23+AF23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="29" t="e">
+        <f aca="false">AVERAGE(F21:F23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" s="29" t="e">
+        <f aca="false">AVERAGE(G21:G23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="29" t="e">
+        <f aca="false">AVERAGE(M21:M23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" s="29" t="e">
+        <f aca="false">AVERAGE(N21:N23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T24" s="29" t="e">
+        <f aca="false">AVERAGE(T21:T23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U24" s="29" t="e">
+        <f aca="false">AVERAGE(U21:U23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA24" s="29" t="e">
+        <f aca="false">AVERAGE(AA21:AA23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB24" s="29" t="e">
+        <f aca="false">AVERAGE(AB21:AB23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH24" s="29" t="e">
+        <f aca="false">AVERAGE(AH21:AH23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI24" s="29" t="e">
+        <f aca="false">AVERAGE(AI21:AI23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="W3:AB3"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="AC5:AC7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="AC9:AC11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="O13:O15"/>
+    <mergeCell ref="V13:V15"/>
+    <mergeCell ref="AC13:AC15"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="O17:O19"/>
+    <mergeCell ref="V17:V19"/>
+    <mergeCell ref="AC17:AC19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="V21:V23"/>
+    <mergeCell ref="AC21:AC23"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>